<commit_message>
doc: Update BOM files
</commit_message>
<xml_diff>
--- a/Hardware/fab/bom/pcb-bolink-batteryHolder.xlsx
+++ b/Hardware/fab/bom/pcb-bolink-batteryHolder.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve"> MPN</t>
   </si>
   <si>
-    <t xml:space="preserve"> ALT_MPN</t>
+    <t xml:space="preserve"> ALT_MPN/Notes</t>
   </si>
   <si>
     <t xml:space="preserve"> Footprint</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">BT1, BT2</t>
   </si>
   <si>
-    <t xml:space="preserve">2xPN57</t>
+    <t xml:space="preserve">PN57</t>
   </si>
   <si>
     <t xml:space="preserve">36-57-ND</t>
@@ -70,37 +70,43 @@
     <t xml:space="preserve">36-69-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Requires THT rework</t>
+  </si>
+  <si>
     <t xml:space="preserve">node-lib-v1:Keystone_69_clip</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.nl/short/zn47d7</t>
   </si>
   <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOLEX PicoBlade 1.25mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_Molex:Molex_PicoBlade_53398-0271_1x02-1MP_P1.25mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_MOLEX_0533980271_MOLEX-0533980271_C122410.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1</t>
   </si>
   <si>
-    <t xml:space="preserve">MOLEX PicoBlade 1.25mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector_Molex:Molex_PicoBlade_53398-0271_1x02-1MP_P1.25mm_Vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_MOLEX_0533980271_MOLEX-0533980271_C122410.html</t>
+    <t xml:space="preserve">DNM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solder 60mm JST-PH Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestPoint:TestPoint_Keystone_5019_Minature</t>
   </si>
   <si>
     <t xml:space="preserve">J2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Keystone_5019_Minature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3</t>
   </si>
   <si>
     <t xml:space="preserve">Part:</t>
@@ -248,15 +254,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,10 +305,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -434,376 +432,375 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL15"/>
+  <dimension ref="A1:BK15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="C3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="7" t="n">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="8" t="n">
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="n">
         <v>533980271</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="H4" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="F5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
+      <c r="E6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="A9" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
+      <c r="A10" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="B10" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
-      <c r="B11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="24" t="n">
-        <f aca="false">SUM(D2:D4)</f>
-        <v>4</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
+      <c r="A11" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="22" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>6</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="24" t="n">
-        <f aca="false">COUNTIF(D2:D4, "&lt;&gt;")</f>
+      <c r="A12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="22" t="n">
+        <f aca="false">COUNTIF(C2:C4, "&lt;&gt;")</f>
         <v>3</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="25"/>
-      <c r="AD12" s="25"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
-      <c r="AI12" s="25"/>
-      <c r="AJ12" s="25"/>
-      <c r="AK12" s="25"/>
-      <c r="AL12" s="25"/>
-      <c r="AM12" s="25"/>
-      <c r="AN12" s="25"/>
-      <c r="AO12" s="25"/>
-      <c r="AP12" s="25"/>
-      <c r="AQ12" s="25"/>
-      <c r="AR12" s="25"/>
-      <c r="AS12" s="25"/>
-      <c r="AT12" s="25"/>
-      <c r="AU12" s="25"/>
-      <c r="AV12" s="25"/>
-      <c r="AW12" s="25"/>
-      <c r="AX12" s="25"/>
-      <c r="AY12" s="25"/>
-      <c r="AZ12" s="25"/>
-      <c r="BA12" s="25"/>
-      <c r="BB12" s="25"/>
-      <c r="BC12" s="25"/>
-      <c r="BD12" s="25"/>
-      <c r="BE12" s="25"/>
-      <c r="BF12" s="25"/>
-      <c r="BG12" s="25"/>
-      <c r="BH12" s="25"/>
-      <c r="BI12" s="25"/>
-      <c r="BJ12" s="25"/>
-      <c r="BK12" s="25"/>
-      <c r="BL12" s="25"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="23"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="23"/>
+      <c r="AI12" s="23"/>
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="23"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="23"/>
+      <c r="AO12" s="23"/>
+      <c r="AP12" s="23"/>
+      <c r="AQ12" s="23"/>
+      <c r="AR12" s="23"/>
+      <c r="AS12" s="23"/>
+      <c r="AT12" s="23"/>
+      <c r="AU12" s="23"/>
+      <c r="AV12" s="23"/>
+      <c r="AW12" s="23"/>
+      <c r="AX12" s="23"/>
+      <c r="AY12" s="23"/>
+      <c r="AZ12" s="23"/>
+      <c r="BA12" s="23"/>
+      <c r="BB12" s="23"/>
+      <c r="BC12" s="23"/>
+      <c r="BD12" s="23"/>
+      <c r="BE12" s="23"/>
+      <c r="BF12" s="23"/>
+      <c r="BG12" s="23"/>
+      <c r="BH12" s="23"/>
+      <c r="BI12" s="23"/>
+      <c r="BJ12" s="23"/>
+      <c r="BK12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
-      <c r="AD13" s="25"/>
-      <c r="AE13" s="25"/>
-      <c r="AF13" s="25"/>
-      <c r="AG13" s="25"/>
-      <c r="AH13" s="25"/>
-      <c r="AI13" s="25"/>
-      <c r="AJ13" s="25"/>
-      <c r="AK13" s="25"/>
-      <c r="AL13" s="25"/>
-      <c r="AM13" s="25"/>
-      <c r="AN13" s="25"/>
-      <c r="AO13" s="25"/>
-      <c r="AP13" s="25"/>
-      <c r="AQ13" s="25"/>
-      <c r="AR13" s="25"/>
-      <c r="AS13" s="25"/>
-      <c r="AT13" s="25"/>
-      <c r="AU13" s="25"/>
-      <c r="AV13" s="25"/>
-      <c r="AW13" s="25"/>
-      <c r="AX13" s="25"/>
-      <c r="AY13" s="25"/>
-      <c r="AZ13" s="25"/>
-      <c r="BA13" s="25"/>
-      <c r="BB13" s="25"/>
-      <c r="BC13" s="25"/>
-      <c r="BD13" s="25"/>
-      <c r="BE13" s="25"/>
-      <c r="BF13" s="25"/>
-      <c r="BG13" s="25"/>
-      <c r="BH13" s="25"/>
-      <c r="BI13" s="25"/>
-      <c r="BJ13" s="25"/>
-      <c r="BK13" s="25"/>
-      <c r="BL13" s="25"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23"/>
+      <c r="AF13" s="23"/>
+      <c r="AG13" s="23"/>
+      <c r="AH13" s="23"/>
+      <c r="AI13" s="23"/>
+      <c r="AJ13" s="23"/>
+      <c r="AK13" s="23"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
+      <c r="AN13" s="23"/>
+      <c r="AO13" s="23"/>
+      <c r="AP13" s="23"/>
+      <c r="AQ13" s="23"/>
+      <c r="AR13" s="23"/>
+      <c r="AS13" s="23"/>
+      <c r="AT13" s="23"/>
+      <c r="AU13" s="23"/>
+      <c r="AV13" s="23"/>
+      <c r="AW13" s="23"/>
+      <c r="AX13" s="23"/>
+      <c r="AY13" s="23"/>
+      <c r="AZ13" s="23"/>
+      <c r="BA13" s="23"/>
+      <c r="BB13" s="23"/>
+      <c r="BC13" s="23"/>
+      <c r="BD13" s="23"/>
+      <c r="BE13" s="23"/>
+      <c r="BF13" s="23"/>
+      <c r="BG13" s="23"/>
+      <c r="BH13" s="23"/>
+      <c r="BI13" s="23"/>
+      <c r="BJ13" s="23"/>
+      <c r="BK13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="A14" s="6"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="26"/>
+      <c r="H15" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://www.digikey.nl/short/zn47d8"/>
-    <hyperlink ref="I3" r:id="rId2" display="https://www.digikey.nl/short/zn47d7"/>
-    <hyperlink ref="I4" r:id="rId3" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_MOLEX_0533980271_MOLEX-0533980271_C122410.html"/>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.digikey.nl/short/zn47d8"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.digikey.nl/short/zn47d7"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://lcsc.com/product-detail/Wire-To-Board-Wire-To-Wire-Connector_MOLEX_0533980271_MOLEX-0533980271_C122410.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>